<commit_message>
Wrote down my justificatoins for lifecycle and updated comments in Ivans files
</commit_message>
<xml_diff>
--- a/IvanAdminUserStories.xlsx
+++ b/IvanAdminUserStories.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan\Desktop\Github\Newsagent-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Palej\Desktop\Software Design with AI for Cloud\Year_3\agile-labs3\Newsagent-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF5C259-2803-48A5-ABD4-AA1B95535747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11DED9CD-4638-44EF-B65D-EA87706549B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="31080" windowHeight="18330" xr2:uid="{FDFDA4C7-506B-4F79-8102-C016FE887AE3}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{FDFDA4C7-506B-4F79-8102-C016FE887AE3}"/>
   </bookViews>
   <sheets>
     <sheet name="AdminUserStories" sheetId="1" r:id="rId1"/>
@@ -39,6 +39,11 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Ivan Lapickij</author>
+    <author>tc={28B74014-11B0-466D-B493-1D2C8C3B8CC7}</author>
+    <author>tc={9C2B62BD-F38F-436A-A248-2A7D791C6D49}</author>
+    <author>tc={6CA07F49-B9F3-483E-B92E-518F30A753E8}</author>
+    <author>tc={FE31F335-F0D5-47E8-A659-EEB9D0447CB9}</author>
+    <author>tc={3DE7F056-8AFB-4F6C-A06F-5190A335B12F}</author>
   </authors>
   <commentList>
     <comment ref="C2" authorId="0" shapeId="0" xr:uid="{F066C8F7-BAE3-480C-97C0-5FD63CF5B79C}">
@@ -63,6 +68,14 @@
           <t xml:space="preserve">
 Is it relevant since there only one admin needed?</t>
         </r>
+      </text>
+    </comment>
+    <comment ref="D2" authorId="1" shapeId="0" xr:uid="{28B74014-11B0-466D-B493-1D2C8C3B8CC7}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    I think relevant unless we assume admin is created by default, idk. I think we need to distinguish between admin acc/delivery acc. But we can for sure discuss</t>
       </text>
     </comment>
     <comment ref="C9" authorId="0" shapeId="0" xr:uid="{5CF9DCC2-56EB-44CE-9BB0-459959AF4B7B}">
@@ -138,6 +151,14 @@
         </r>
       </text>
     </comment>
+    <comment ref="D33" authorId="2" shapeId="0" xr:uid="{9C2B62BD-F38F-436A-A248-2A7D791C6D49}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This isnt a new role. You wont say "as a system I want to…", because system is not a WHO. You want to personalize it, so we can say "system manager" instead which literally is the same as "system". Admin only deals with Create/Delete/Read/Print/Update - allowing for these options. Then someone else uses them, that’s my  thinking</t>
+      </text>
+    </comment>
     <comment ref="C43" authorId="0" shapeId="0" xr:uid="{453218D5-992A-43DA-994B-93185F6212D7}">
       <text>
         <r>
@@ -151,6 +172,14 @@
           <t>Ivan Lapickij
 update status maybe as a admin? Cuz this is new feature that client didn’t ask "deactivate"</t>
         </r>
+      </text>
+    </comment>
+    <comment ref="D43" authorId="3" shapeId="0" xr:uid="{6CA07F49-B9F3-483E-B92E-518F30A753E8}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    We can discuss that as to me this represents the requirement when the customer does not want to subscribe for certain amount of time?</t>
       </text>
     </comment>
     <comment ref="B53" authorId="0" shapeId="0" xr:uid="{5F945C8A-FEB1-4F7D-A4B1-145FCF2EF972}">
@@ -175,6 +204,23 @@
           <t xml:space="preserve">
 New role or admin?</t>
         </r>
+      </text>
+    </comment>
+    <comment ref="C53" authorId="4" shapeId="0" xr:uid="{FE31F335-F0D5-47E8-A659-EEB9D0447CB9}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    I think new role as Ronan mentioned in one of his whatsapp messages before - adding entity will break down the workload for the ones we already have decided on
+</t>
+      </text>
+    </comment>
+    <comment ref="B72" authorId="5" shapeId="0" xr:uid="{3DE7F056-8AFB-4F6C-A06F-5190A335B12F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Im not sure whats meant by that</t>
       </text>
     </comment>
   </commentList>
@@ -708,32 +754,81 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -744,55 +839,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -814,6 +860,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Natalia Palej" id="{1BDC7653-6475-40D8-8DEF-03772E9AD5E4}" userId="cad1acabf18afac6" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1111,25 +1163,46 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="D2" dT="2023-10-01T17:38:25.98" personId="{1BDC7653-6475-40D8-8DEF-03772E9AD5E4}" id="{28B74014-11B0-466D-B493-1D2C8C3B8CC7}">
+    <text>I think relevant unless we assume admin is created by default, idk. I think we need to distinguish between admin acc/delivery acc. But we can for sure discuss</text>
+  </threadedComment>
+  <threadedComment ref="D33" dT="2023-10-01T17:37:26.92" personId="{1BDC7653-6475-40D8-8DEF-03772E9AD5E4}" id="{9C2B62BD-F38F-436A-A248-2A7D791C6D49}">
+    <text>This isnt a new role. You wont say "as a system I want to…", because system is not a WHO. You want to personalize it, so we can say "system manager" instead which literally is the same as "system". Admin only deals with Create/Delete/Read/Print/Update - allowing for these options. Then someone else uses them, that’s my  thinking</text>
+  </threadedComment>
+  <threadedComment ref="D43" dT="2023-10-01T17:35:37.07" personId="{1BDC7653-6475-40D8-8DEF-03772E9AD5E4}" id="{6CA07F49-B9F3-483E-B92E-518F30A753E8}">
+    <text>We can discuss that as to me this represents the requirement when the customer does not want to subscribe for certain amount of time?</text>
+  </threadedComment>
+  <threadedComment ref="C53" dT="2023-10-01T17:39:16.16" personId="{1BDC7653-6475-40D8-8DEF-03772E9AD5E4}" id="{FE31F335-F0D5-47E8-A659-EEB9D0447CB9}">
+    <text xml:space="preserve">I think new role as Ronan mentioned in one of his whatsapp messages before - adding entity will break down the workload for the ones we already have decided on
+</text>
+  </threadedComment>
+  <threadedComment ref="B72" dT="2023-10-01T17:39:47.94" personId="{1BDC7653-6475-40D8-8DEF-03772E9AD5E4}" id="{3DE7F056-8AFB-4F6C-A06F-5190A335B12F}">
+    <text>Im not sure whats meant by that</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AB095BD-E922-497D-B7ED-398078A18E3D}">
   <dimension ref="A1:F72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53:B55"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="3" max="3" width="31.7109375" customWidth="1"/>
+    <col min="1" max="1" width="2.86328125" customWidth="1"/>
+    <col min="2" max="2" width="13.1328125" customWidth="1"/>
+    <col min="3" max="3" width="31.73046875" customWidth="1"/>
     <col min="4" max="4" width="38" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="81" style="16" customWidth="1"/>
-    <col min="6" max="6" width="63.7109375" customWidth="1"/>
+    <col min="6" max="6" width="63.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>1</v>
@@ -1147,17 +1220,17 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="28">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="26">
         <v>13</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="28" t="s">
         <v>50</v>
       </c>
       <c r="E2" s="20" t="s">
@@ -1167,11 +1240,11 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="29"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="26"/>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="27"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="29"/>
       <c r="E3" s="20" t="s">
         <v>69</v>
       </c>
@@ -1179,47 +1252,47 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="29"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="26"/>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="27"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="29"/>
       <c r="E4" s="20" t="s">
         <v>71</v>
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="29"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="43"/>
-      <c r="D5" s="26"/>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="27"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="29"/>
       <c r="E5" s="20" t="s">
         <v>72</v>
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="29"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="26"/>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="27"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="29"/>
       <c r="E6" s="20" t="s">
         <v>56</v>
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="29"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="26"/>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="27"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="29"/>
       <c r="E7" s="20" t="s">
         <v>48</v>
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="6"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
@@ -1227,17 +1300,17 @@
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="28">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="26">
         <v>1</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="28" t="s">
         <v>5</v>
       </c>
       <c r="E9" s="19" t="s">
@@ -1245,87 +1318,87 @@
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="43"/>
-      <c r="D10" s="26"/>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="27"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="29"/>
       <c r="E10" s="20" t="s">
         <v>82</v>
       </c>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="43"/>
-      <c r="D11" s="26"/>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="27"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="29"/>
       <c r="E11" s="20" t="s">
         <v>65</v>
       </c>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="29"/>
-      <c r="B12" s="26"/>
-      <c r="C12" s="43"/>
-      <c r="D12" s="26"/>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" s="27"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="29"/>
       <c r="E12" s="20" t="s">
         <v>64</v>
       </c>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="43"/>
-      <c r="D13" s="26"/>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" s="27"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="29"/>
       <c r="E13" s="20" t="s">
         <v>66</v>
       </c>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="29"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="43"/>
-      <c r="D14" s="26"/>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" s="27"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="29"/>
       <c r="E14" s="20" t="s">
         <v>67</v>
       </c>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="29"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="43"/>
-      <c r="D15" s="26"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15" s="27"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="29"/>
       <c r="E15" s="20" t="s">
         <v>83</v>
       </c>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="29"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="26"/>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" s="27"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="29"/>
       <c r="E16" s="20" t="s">
         <v>84</v>
       </c>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="30"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="44"/>
-      <c r="D17" s="27"/>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17" s="46"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="47"/>
       <c r="E17" s="20" t="s">
         <v>16</v>
       </c>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="3"/>
       <c r="B18" s="13"/>
       <c r="C18" s="13"/>
@@ -1333,17 +1406,17 @@
       <c r="E18" s="21"/>
       <c r="F18" s="12"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="28">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19" s="26">
         <v>2</v>
       </c>
-      <c r="B19" s="25" t="s">
+      <c r="B19" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="25" t="s">
+      <c r="C19" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="25" t="s">
+      <c r="D19" s="28" t="s">
         <v>7</v>
       </c>
       <c r="E19" s="20" t="s">
@@ -1353,27 +1426,27 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="29"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20" s="27"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
       <c r="E20" s="20" t="s">
         <v>46</v>
       </c>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="30"/>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A21" s="46"/>
+      <c r="B21" s="47"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="47"/>
       <c r="E21" s="16" t="s">
         <v>73</v>
       </c>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="3"/>
       <c r="B22" s="13"/>
       <c r="C22" s="13"/>
@@ -1381,17 +1454,17 @@
       <c r="E22" s="21"/>
       <c r="F22" s="12"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="28">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A23" s="26">
         <v>3</v>
       </c>
-      <c r="B23" s="25" t="s">
+      <c r="B23" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="C23" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="D23" s="25" t="s">
+      <c r="D23" s="28" t="s">
         <v>10</v>
       </c>
       <c r="E23" s="20" t="s">
@@ -1401,27 +1474,27 @@
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="29"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24" s="27"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
       <c r="E24" s="20" t="s">
         <v>39</v>
       </c>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="30"/>
-      <c r="B25" s="27"/>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27"/>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A25" s="46"/>
+      <c r="B25" s="47"/>
+      <c r="C25" s="47"/>
+      <c r="D25" s="47"/>
       <c r="E25" s="20" t="s">
         <v>11</v>
       </c>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="3"/>
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
@@ -1429,17 +1502,17 @@
       <c r="E26" s="21"/>
       <c r="F26" s="12"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="28">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A27" s="26">
         <v>4</v>
       </c>
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C27" s="25" t="s">
+      <c r="C27" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="25" t="s">
+      <c r="D27" s="28" t="s">
         <v>12</v>
       </c>
       <c r="E27" s="20" t="s">
@@ -1447,17 +1520,17 @@
       </c>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="30"/>
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A28" s="46"/>
+      <c r="B28" s="47"/>
+      <c r="C28" s="47"/>
+      <c r="D28" s="47"/>
       <c r="E28" s="20" t="s">
         <v>15</v>
       </c>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="3"/>
       <c r="B29" s="13"/>
       <c r="C29" s="13"/>
@@ -1465,17 +1538,17 @@
       <c r="E29" s="21"/>
       <c r="F29" s="12"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="28">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A30" s="26">
         <v>5</v>
       </c>
-      <c r="B30" s="25" t="s">
+      <c r="B30" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C30" s="25" t="s">
+      <c r="C30" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="D30" s="25" t="s">
+      <c r="D30" s="28" t="s">
         <v>18</v>
       </c>
       <c r="E30" s="20" t="s">
@@ -1485,17 +1558,17 @@
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="30"/>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A31" s="46"/>
+      <c r="B31" s="47"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="47"/>
       <c r="E31" s="20" t="s">
         <v>20</v>
       </c>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="6"/>
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
@@ -1503,17 +1576,17 @@
       <c r="E32" s="12"/>
       <c r="F32" s="12"/>
     </row>
-    <row r="33" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="37">
         <v>12</v>
       </c>
-      <c r="B33" s="42" t="s">
+      <c r="B33" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="C33" s="42" t="s">
+      <c r="C33" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="D33" s="31" t="s">
+      <c r="D33" s="34" t="s">
         <v>54</v>
       </c>
       <c r="E33" s="22" t="s">
@@ -1521,37 +1594,37 @@
       </c>
       <c r="F33" s="10"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" s="38"/>
-      <c r="B34" s="43"/>
-      <c r="C34" s="43"/>
-      <c r="D34" s="32"/>
+      <c r="B34" s="31"/>
+      <c r="C34" s="31"/>
+      <c r="D34" s="35"/>
       <c r="E34" s="22" t="s">
         <v>52</v>
       </c>
       <c r="F34" s="10"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="38"/>
-      <c r="B35" s="43"/>
-      <c r="C35" s="43"/>
-      <c r="D35" s="32"/>
+      <c r="B35" s="31"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="35"/>
       <c r="E35" s="22" t="s">
         <v>47</v>
       </c>
       <c r="F35" s="10"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="39"/>
-      <c r="B36" s="44"/>
-      <c r="C36" s="44"/>
-      <c r="D36" s="33"/>
+      <c r="B36" s="48"/>
+      <c r="C36" s="48"/>
+      <c r="D36" s="36"/>
       <c r="E36" s="22" t="s">
         <v>48</v>
       </c>
       <c r="F36" s="10"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="6"/>
       <c r="B37" s="12"/>
       <c r="C37" s="12"/>
@@ -1559,17 +1632,17 @@
       <c r="E37" s="12"/>
       <c r="F37" s="12"/>
     </row>
-    <row r="38" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="37">
         <v>12</v>
       </c>
-      <c r="B38" s="34" t="s">
+      <c r="B38" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="C38" s="34" t="s">
+      <c r="C38" s="51" t="s">
         <v>86</v>
       </c>
-      <c r="D38" s="31" t="s">
+      <c r="D38" s="34" t="s">
         <v>54</v>
       </c>
       <c r="E38" s="22" t="s">
@@ -1577,37 +1650,37 @@
       </c>
       <c r="F38" s="10"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="38"/>
-      <c r="B39" s="35"/>
-      <c r="C39" s="35"/>
-      <c r="D39" s="32"/>
+      <c r="B39" s="52"/>
+      <c r="C39" s="52"/>
+      <c r="D39" s="35"/>
       <c r="E39" s="22" t="s">
         <v>52</v>
       </c>
       <c r="F39" s="10"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="38"/>
-      <c r="B40" s="35"/>
-      <c r="C40" s="35"/>
-      <c r="D40" s="32"/>
+      <c r="B40" s="52"/>
+      <c r="C40" s="52"/>
+      <c r="D40" s="35"/>
       <c r="E40" s="22" t="s">
         <v>47</v>
       </c>
       <c r="F40" s="10"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" s="39"/>
-      <c r="B41" s="36"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="33"/>
+      <c r="B41" s="53"/>
+      <c r="C41" s="53"/>
+      <c r="D41" s="36"/>
       <c r="E41" s="22" t="s">
         <v>48</v>
       </c>
       <c r="F41" s="10"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" s="2"/>
       <c r="B42" s="14"/>
       <c r="C42" s="14"/>
@@ -1615,17 +1688,17 @@
       <c r="E42" s="21"/>
       <c r="F42" s="12"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" s="37">
         <v>8</v>
       </c>
-      <c r="B43" s="31" t="s">
+      <c r="B43" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="34" t="s">
+      <c r="C43" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="D43" s="31" t="s">
+      <c r="D43" s="34" t="s">
         <v>61</v>
       </c>
       <c r="E43" s="23" t="s">
@@ -1633,47 +1706,47 @@
       </c>
       <c r="F43" s="10"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" s="38"/>
-      <c r="B44" s="32"/>
-      <c r="C44" s="35"/>
-      <c r="D44" s="32"/>
+      <c r="B44" s="35"/>
+      <c r="C44" s="52"/>
+      <c r="D44" s="35"/>
       <c r="E44" s="22" t="s">
         <v>27</v>
       </c>
       <c r="F44" s="10"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="38"/>
-      <c r="B45" s="32"/>
-      <c r="C45" s="35"/>
-      <c r="D45" s="32"/>
+      <c r="B45" s="35"/>
+      <c r="C45" s="52"/>
+      <c r="D45" s="35"/>
       <c r="E45" s="22" t="s">
         <v>28</v>
       </c>
       <c r="F45" s="10"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" s="38"/>
-      <c r="B46" s="32"/>
-      <c r="C46" s="35"/>
-      <c r="D46" s="32"/>
+      <c r="B46" s="35"/>
+      <c r="C46" s="52"/>
+      <c r="D46" s="35"/>
       <c r="E46" s="22" t="s">
         <v>29</v>
       </c>
       <c r="F46" s="10"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" s="39"/>
-      <c r="B47" s="33"/>
-      <c r="C47" s="36"/>
-      <c r="D47" s="33"/>
+      <c r="B47" s="36"/>
+      <c r="C47" s="53"/>
+      <c r="D47" s="36"/>
       <c r="E47" s="22" t="s">
         <v>25</v>
       </c>
       <c r="F47" s="10"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" s="3"/>
       <c r="B48" s="13"/>
       <c r="C48" s="13"/>
@@ -1681,17 +1754,17 @@
       <c r="E48" s="21"/>
       <c r="F48" s="12"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" s="37">
         <v>9</v>
       </c>
-      <c r="B49" s="31" t="s">
+      <c r="B49" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="C49" s="31" t="s">
+      <c r="C49" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="D49" s="31" t="s">
+      <c r="D49" s="34" t="s">
         <v>31</v>
       </c>
       <c r="E49" s="22" t="s">
@@ -1699,27 +1772,27 @@
       </c>
       <c r="F49" s="10"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" s="38"/>
-      <c r="B50" s="32"/>
-      <c r="C50" s="32"/>
-      <c r="D50" s="32"/>
+      <c r="B50" s="35"/>
+      <c r="C50" s="35"/>
+      <c r="D50" s="35"/>
       <c r="E50" s="22" t="s">
         <v>43</v>
       </c>
       <c r="F50" s="10"/>
     </row>
-    <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A51" s="39"/>
-      <c r="B51" s="33"/>
-      <c r="C51" s="33"/>
-      <c r="D51" s="33"/>
+      <c r="B51" s="36"/>
+      <c r="C51" s="36"/>
+      <c r="D51" s="36"/>
       <c r="E51" s="22" t="s">
         <v>44</v>
       </c>
       <c r="F51" s="10"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" s="3"/>
       <c r="B52" s="13"/>
       <c r="C52" s="13"/>
@@ -1727,45 +1800,45 @@
       <c r="E52" s="21"/>
       <c r="F52" s="12"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="45">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A53" s="40">
         <v>10</v>
       </c>
-      <c r="B53" s="42" t="s">
+      <c r="B53" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="C53" s="48" t="s">
+      <c r="C53" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="D53" s="48" t="s">
+      <c r="D53" s="43" t="s">
         <v>41</v>
       </c>
       <c r="E53" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="F53" s="40" t="s">
+      <c r="F53" s="49" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="46"/>
-      <c r="B54" s="43"/>
-      <c r="C54" s="49"/>
-      <c r="D54" s="49"/>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A54" s="41"/>
+      <c r="B54" s="31"/>
+      <c r="C54" s="44"/>
+      <c r="D54" s="44"/>
       <c r="E54" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="F54" s="41"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="47"/>
-      <c r="B55" s="44"/>
-      <c r="C55" s="50"/>
-      <c r="D55" s="50"/>
+      <c r="F54" s="50"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A55" s="42"/>
+      <c r="B55" s="48"/>
+      <c r="C55" s="45"/>
+      <c r="D55" s="45"/>
       <c r="E55" s="11"/>
       <c r="F55" s="11"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56" s="3"/>
       <c r="B56" s="13"/>
       <c r="C56" s="13"/>
@@ -1773,17 +1846,17 @@
       <c r="E56" s="21"/>
       <c r="F56" s="12"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="45">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A57" s="40">
         <v>11</v>
       </c>
-      <c r="B57" s="48" t="s">
+      <c r="B57" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="C57" s="48" t="s">
+      <c r="C57" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="D57" s="48" t="s">
+      <c r="D57" s="43" t="s">
         <v>33</v>
       </c>
       <c r="E57" s="24" t="s">
@@ -1791,67 +1864,67 @@
       </c>
       <c r="F57" s="11"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="46"/>
-      <c r="B58" s="49"/>
-      <c r="C58" s="49"/>
-      <c r="D58" s="49"/>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A58" s="41"/>
+      <c r="B58" s="44"/>
+      <c r="C58" s="44"/>
+      <c r="D58" s="44"/>
       <c r="E58" s="24" t="s">
         <v>35</v>
       </c>
       <c r="F58" s="11"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="47"/>
-      <c r="B59" s="50"/>
-      <c r="C59" s="50"/>
-      <c r="D59" s="50"/>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A59" s="42"/>
+      <c r="B59" s="45"/>
+      <c r="C59" s="45"/>
+      <c r="D59" s="45"/>
       <c r="E59" s="24" t="s">
         <v>36</v>
       </c>
       <c r="F59" s="11"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
       <c r="E62" s="14"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="51">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A63" s="32">
         <v>6</v>
       </c>
-      <c r="B63" s="51" t="s">
+      <c r="B63" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C63" s="51" t="s">
+      <c r="C63" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="D63" s="51" t="s">
+      <c r="D63" s="32" t="s">
         <v>22</v>
       </c>
       <c r="E63" s="17" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="52"/>
-      <c r="B64" s="52"/>
-      <c r="C64" s="52"/>
-      <c r="D64" s="52"/>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A64" s="33"/>
+      <c r="B64" s="33"/>
+      <c r="C64" s="33"/>
+      <c r="D64" s="33"/>
       <c r="E64" s="17" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
       <c r="E65" s="14"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A66" s="7">
         <v>7</v>
       </c>
@@ -1868,7 +1941,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A67" s="8"/>
       <c r="B67" s="8"/>
       <c r="C67" s="8"/>
@@ -1877,7 +1950,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A68" s="8"/>
       <c r="B68" s="8"/>
       <c r="C68" s="8"/>
@@ -1886,7 +1959,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A69" s="9"/>
       <c r="B69" s="9"/>
       <c r="C69" s="9"/>
@@ -1895,26 +1968,63 @@
         <v>25</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
       <c r="E70" s="14"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B72" s="53" t="s">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B72" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="C72" s="53" t="s">
+      <c r="C72" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="D72" s="53" t="s">
+      <c r="D72" s="25" t="s">
         <v>88</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="53">
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="F53:F54"/>
+    <mergeCell ref="A33:A36"/>
+    <mergeCell ref="B33:B36"/>
+    <mergeCell ref="C33:C36"/>
+    <mergeCell ref="D33:D36"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="C53:C55"/>
+    <mergeCell ref="D53:D55"/>
+    <mergeCell ref="D43:D47"/>
+    <mergeCell ref="C43:C47"/>
+    <mergeCell ref="B43:B47"/>
+    <mergeCell ref="A43:A47"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="C38:C41"/>
+    <mergeCell ref="D38:D41"/>
+    <mergeCell ref="A9:A17"/>
+    <mergeCell ref="B9:B17"/>
+    <mergeCell ref="C9:C17"/>
+    <mergeCell ref="D9:D17"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="A19:A21"/>
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="B2:B7"/>
     <mergeCell ref="C2:C7"/>
@@ -1931,43 +2041,6 @@
     <mergeCell ref="B57:B59"/>
     <mergeCell ref="C57:C59"/>
     <mergeCell ref="D57:D59"/>
-    <mergeCell ref="A9:A17"/>
-    <mergeCell ref="B9:B17"/>
-    <mergeCell ref="C9:C17"/>
-    <mergeCell ref="D9:D17"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="F53:F54"/>
-    <mergeCell ref="A33:A36"/>
-    <mergeCell ref="B33:B36"/>
-    <mergeCell ref="C33:C36"/>
-    <mergeCell ref="D33:D36"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="C53:C55"/>
-    <mergeCell ref="D53:D55"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="D43:D47"/>
-    <mergeCell ref="C43:C47"/>
-    <mergeCell ref="B43:B47"/>
-    <mergeCell ref="A43:A47"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="C38:C41"/>
-    <mergeCell ref="D38:D41"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>